<commit_message>
update at harness master
update at harness master
</commit_message>
<xml_diff>
--- a/wiring_connections.xlsx
+++ b/wiring_connections.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c3132704\Documents\GitHub\NU-Racing---ETC-and-manumatic-Electronics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="23940" windowHeight="15060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="conns" sheetId="1" r:id="rId1"/>
     <sheet name="connectors" sheetId="2" r:id="rId2"/>
+    <sheet name="LOOKUP" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">connectors!$A$1:$H$49</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="98">
   <si>
     <t>GS MODULE</t>
   </si>
@@ -132,9 +131,6 @@
     <t>DEST</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>DTM</t>
   </si>
   <si>
@@ -156,12 +152,6 @@
     <t>ECU</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>DTHD</t>
   </si>
   <si>
@@ -225,9 +215,6 @@
     <t>MODE_KN</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>MODULE</t>
   </si>
   <si>
@@ -289,13 +276,58 @@
   </si>
   <si>
     <t>POSS CONS</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Additional DS button on clutch post</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>GREY</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>BRN</t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t>BLUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +339,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,8 +437,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -409,7 +459,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,7 +520,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,7 +555,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -680,7 +732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,18 +746,18 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="51.75" customHeight="1">
       <c r="B1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -717,13 +769,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -735,7 +787,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -747,7 +799,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -759,7 +811,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -771,7 +823,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -783,37 +835,37 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="D15" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -825,7 +877,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -837,7 +889,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -852,7 +904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -864,13 +916,13 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -882,7 +934,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -894,7 +946,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -909,7 +961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -921,16 +973,16 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -947,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -964,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -981,7 +1033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -998,7 +1050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1046,7 +1098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1063,36 +1115,41 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1103,1014 +1160,1329 @@
         <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
         <v>67</v>
       </c>
-      <c r="G13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f>VLOOKUP(I18,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+      <c r="K18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f>VLOOKUP(I19,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+      <c r="K19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f>VLOOKUP(I20,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+      <c r="K20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f>VLOOKUP(I21,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+      <c r="K21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B22">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22">
+        <f>VLOOKUP(I22,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B23">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23">
+        <f>VLOOKUP(I23,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B24">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>85</v>
+      </c>
+      <c r="J24">
+        <f>VLOOKUP(I24,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B25">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I25" t="s">
+        <v>86</v>
+      </c>
+      <c r="J25">
+        <f>VLOOKUP(I25,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B26">
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E26" s="10">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I26" t="s">
+        <v>86</v>
+      </c>
+      <c r="J26">
+        <f>VLOOKUP(I26,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E28" s="10">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I28" t="s">
+        <v>86</v>
+      </c>
+      <c r="J28">
+        <f>VLOOKUP(I28,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E29" s="10">
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I29" t="s">
+        <v>86</v>
+      </c>
+      <c r="J29">
+        <f>VLOOKUP(I29,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I30" t="s">
+        <v>86</v>
+      </c>
+      <c r="J30">
+        <f>VLOOKUP(I30,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="J31">
+        <v>2000</v>
+      </c>
+      <c r="K31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="J32">
+        <v>2000</v>
+      </c>
+      <c r="K32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33">
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33">
+        <f>VLOOKUP(I33,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I34" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34">
+        <f>VLOOKUP(I34,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I35" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35">
+        <f>VLOOKUP(I35,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K35" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I36" t="s">
+        <v>86</v>
+      </c>
+      <c r="J36">
+        <f>VLOOKUP(I36,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="K36" t="s">
+        <v>87</v>
+      </c>
+      <c r="M36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G37" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <f>VLOOKUP(I37,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+      <c r="K37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G38" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f>VLOOKUP(I38,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+      <c r="K38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39">
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G39" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f>VLOOKUP(I39,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G41" t="s">
+        <v>81</v>
+      </c>
+      <c r="I41" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J41" s="7">
+        <f>VLOOKUP(I41,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
         <v>44</v>
       </c>
-      <c r="D42" t="s">
-        <v>47</v>
-      </c>
       <c r="E42" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G42" t="s">
+        <v>81</v>
+      </c>
+      <c r="I42" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J42" s="7">
+        <f>VLOOKUP(I42,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G43" t="s">
+        <v>81</v>
+      </c>
+      <c r="I43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J43" s="7">
+        <f>VLOOKUP(I43,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G46" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>85</v>
+      </c>
+      <c r="J46" s="7">
+        <f>VLOOKUP(I46,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E47" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" t="s">
+        <v>81</v>
+      </c>
+      <c r="I47" t="s">
+        <v>85</v>
+      </c>
+      <c r="J47" s="7">
+        <f>VLOOKUP(I47,LOOKUP!$A$1:$B$3,2,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="K47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="F47" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
       <c r="B49">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>1500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>